<commit_message>
More debug data. Compatible w occ opt 4.1 BETA
All of the actual datasets stayed the same.
</commit_message>
<xml_diff>
--- a/EnergyPlusOpt2Fed/EnergyPlusOpt2Fed_deployment/WholesalePrice.xlsx
+++ b/EnergyPlusOpt2Fed/EnergyPlusOpt2Fed_deployment/WholesalePrice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Jan1thru7" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,10 @@
     <sheet name="bugoff" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="bugfreeze" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="bugcook" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="bugsnug" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="bugwarm" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="bugAC" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="bughprice" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -143,11 +147,11 @@
   </sheetPr>
   <dimension ref="A1:A2053"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2020" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2016" activeCellId="0" sqref="A2016"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1747" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2016" activeCellId="1" sqref="A4:A16 A2016"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10433,7 +10437,7 @@
   <dimension ref="A2:C2065"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="A4:A16 G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29044,10 +29048,10 @@
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A4:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -29056,137 +29060,159 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A2-4</f>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A3-4</f>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A4-4</f>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A5-4</f>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A6-4</f>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>20</v>
+        <f aca="false">A7-4</f>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A8-4</f>
+        <v>72</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A9-4</f>
+        <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A10-4</f>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A11-4</f>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A12-4</f>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A13-4</f>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A14-4</f>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A15-4</f>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A16-4</f>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A17-4</f>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A18-4</f>
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A19-4</f>
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A20-4</f>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A21-4</f>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A22-4</f>
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>99</v>
+        <f aca="false">A23-4</f>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -29208,10 +29234,10 @@
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="1" sqref="A4:A16 A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -29394,13 +29420,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:A16 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -29429,7 +29455,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29439,22 +29465,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>99</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29469,72 +29495,733 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>150</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A4:A16 B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A4:A16 B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Occupancy Optimization v5.0 Stable
</commit_message>
<xml_diff>
--- a/EnergyPlusOpt2Fed/EnergyPlusOpt2Fed_deployment/WholesalePrice.xlsx
+++ b/EnergyPlusOpt2Fed/EnergyPlusOpt2Fed_deployment/WholesalePrice.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Jan1thru7" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Feb12thru19" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sept27thruOct3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sep27-Oct3_SJ" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="bugoff" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="bugfreeze" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="bugcook" sheetId="6" state="visible" r:id="rId7"/>
@@ -41,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -68,11 +68,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,7 +112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -132,10 +127,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -161,7 +152,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -10450,7 +10441,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -29225,13 +29216,13 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -40777,7 +40768,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -40963,7 +40954,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -41152,7 +41143,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -41316,7 +41307,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -41480,7 +41471,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -41644,7 +41635,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>